<commit_message>
✅ add csv and xlsx parsing and tests
</commit_message>
<xml_diff>
--- a/test/data/IPSSMexample.xlsx
+++ b/test/data/IPSSMexample.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernare2/Documents/postdoc/iwg_mds/src/Analysis/story/210510/calculator/viii5/devRpackage/ipssm/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arangooj/projects/ipssm/ipssm-js/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51056280-4990-FC44-B27F-CFB39FCCB1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E469B92-17FB-7E4A-834A-F2E84ECF1F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36080" yWindow="4840" windowWidth="34920" windowHeight="21140" activeTab="1" xr2:uid="{14BB6C89-D464-5645-B38C-0AC87AAACFC4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{14BB6C89-D464-5645-B38C-0AC87AAACFC4}"/>
   </bookViews>
   <sheets>
-    <sheet name="explain" sheetId="1" r:id="rId1"/>
-    <sheet name="examples" sheetId="2" r:id="rId2"/>
+    <sheet name="examples" sheetId="2" r:id="rId1"/>
+    <sheet name="explain" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="86">
   <si>
     <t>category</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>numerical, between 0 and 1</t>
+  </si>
+  <si>
+    <t>ANC</t>
+  </si>
+  <si>
+    <t>AGE</t>
   </si>
 </sst>
 </file>
@@ -725,11 +731,428 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337C1B46-DC91-CB42-979E-0AEDD11D90E3}">
+  <dimension ref="A1:AR3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:44" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR1" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="9">
+        <v>9.6</v>
+      </c>
+      <c r="C2">
+        <v>281</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>4.84</v>
+      </c>
+      <c r="F2">
+        <v>79</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>0.24</v>
+      </c>
+      <c r="F3">
+        <v>66</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09DA4B4D-FC9D-5441-A1A8-6A6AB959E6D1}">
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1415,401 +1838,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337C1B46-DC91-CB42-979E-0AEDD11D90E3}">
-  <dimension ref="A1:AP3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:42" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="W1" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y1" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA1" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB1" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM1" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN1" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO1" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="AP1" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="9">
-        <v>9.6</v>
-      </c>
-      <c r="C2">
-        <v>281</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2">
-        <v>1</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ2" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL2" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="9">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO2" s="9">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="C3">
-        <v>23</v>
-      </c>
-      <c r="D3">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="9">
-        <v>0.85</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
🐛 fix SF3B1alpha conditions
</commit_message>
<xml_diff>
--- a/test/data/IPSSMexample.xlsx
+++ b/test/data/IPSSMexample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arangooj/projects/ipssm/ipssm-js/test/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arangooj/papaemme/ipssm-api/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E469B92-17FB-7E4A-834A-F2E84ECF1F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F663D2-4CBA-3D45-845F-9E46803F60EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{14BB6C89-D464-5645-B38C-0AC87AAACFC4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="examples" sheetId="2" r:id="rId1"/>
     <sheet name="explain" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="91">
   <si>
     <t>category</t>
   </si>
@@ -293,6 +293,21 @@
   </si>
   <si>
     <t>AGE</t>
+  </si>
+  <si>
+    <t>withNAs</t>
+  </si>
+  <si>
+    <t>SF3B1alphaTestCase</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>zeroScore</t>
+  </si>
+  <si>
+    <t>Very Good</t>
   </si>
 </sst>
 </file>
@@ -732,15 +747,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337C1B46-DC91-CB42-979E-0AEDD11D90E3}">
-  <dimension ref="A1:AR3"/>
+  <dimension ref="A1:CW13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:44" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:101" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>68</v>
       </c>
@@ -874,7 +889,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
@@ -1008,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>71</v>
       </c>
@@ -1141,6 +1156,666 @@
       <c r="AR3" s="9">
         <v>0</v>
       </c>
+    </row>
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="9">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="9"/>
+      <c r="AT4" s="9"/>
+      <c r="BB4" s="9"/>
+      <c r="BE4" s="9"/>
+      <c r="CC4" s="9"/>
+      <c r="CD4" s="9"/>
+      <c r="CE4" s="9"/>
+      <c r="CF4" s="9"/>
+      <c r="CG4" s="9"/>
+      <c r="CH4" s="9"/>
+      <c r="CI4" s="9"/>
+      <c r="CJ4" s="9"/>
+      <c r="CK4" s="9"/>
+      <c r="CL4" s="9"/>
+      <c r="CT4" s="9"/>
+      <c r="CW4" s="9"/>
+    </row>
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="9">
+        <v>9.6</v>
+      </c>
+      <c r="C5">
+        <v>281</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>4.84</v>
+      </c>
+      <c r="F5">
+        <v>79</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AS5" s="9"/>
+      <c r="AT5" s="9"/>
+      <c r="BB5" s="9"/>
+      <c r="BE5" s="9"/>
+      <c r="CC5" s="9"/>
+      <c r="CD5" s="9"/>
+      <c r="CE5" s="9"/>
+      <c r="CF5" s="9"/>
+      <c r="CG5" s="9"/>
+      <c r="CH5" s="9"/>
+      <c r="CI5" s="9"/>
+      <c r="CJ5" s="9"/>
+      <c r="CK5" s="9"/>
+      <c r="CL5" s="9"/>
+      <c r="CT5" s="9"/>
+      <c r="CW5" s="9"/>
+    </row>
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="9">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="BB6" s="9"/>
+      <c r="BE6" s="9"/>
+      <c r="CC6" s="9"/>
+      <c r="CD6" s="9"/>
+      <c r="CE6" s="9"/>
+      <c r="CF6" s="9"/>
+      <c r="CG6" s="9"/>
+      <c r="CH6" s="9"/>
+      <c r="CI6" s="9"/>
+      <c r="CJ6" s="9"/>
+      <c r="CK6" s="9"/>
+      <c r="CL6" s="9"/>
+      <c r="CT6" s="9"/>
+      <c r="CW6" s="9"/>
+    </row>
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="BB7" s="9"/>
+      <c r="BE7" s="9"/>
+      <c r="CC7" s="9"/>
+      <c r="CD7" s="9"/>
+      <c r="CE7" s="9"/>
+      <c r="CF7" s="9"/>
+      <c r="CG7" s="9"/>
+      <c r="CH7" s="9"/>
+      <c r="CI7" s="9"/>
+      <c r="CJ7" s="9"/>
+      <c r="CK7" s="9"/>
+      <c r="CL7" s="9"/>
+      <c r="CT7" s="9"/>
+      <c r="CW7" s="9"/>
+    </row>
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="BB8" s="9"/>
+      <c r="BE8" s="9"/>
+      <c r="CC8" s="9"/>
+      <c r="CD8" s="9"/>
+      <c r="CE8" s="9"/>
+      <c r="CF8" s="9"/>
+      <c r="CG8" s="9"/>
+      <c r="CH8" s="9"/>
+      <c r="CI8" s="9"/>
+      <c r="CJ8" s="9"/>
+      <c r="CK8" s="9"/>
+      <c r="CL8" s="9"/>
+      <c r="CT8" s="9"/>
+      <c r="CW8" s="9"/>
+    </row>
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="BB9" s="9"/>
+      <c r="BE9" s="9"/>
+      <c r="CC9" s="9"/>
+      <c r="CD9" s="9"/>
+      <c r="CE9" s="9"/>
+      <c r="CF9" s="9"/>
+      <c r="CG9" s="9"/>
+      <c r="CH9" s="9"/>
+      <c r="CI9" s="9"/>
+      <c r="CJ9" s="9"/>
+      <c r="CK9" s="9"/>
+      <c r="CL9" s="9"/>
+      <c r="CT9" s="9"/>
+      <c r="CW9" s="9"/>
+    </row>
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="BB10" s="9"/>
+      <c r="BE10" s="9"/>
+      <c r="CC10" s="9"/>
+      <c r="CD10" s="9"/>
+      <c r="CE10" s="9"/>
+      <c r="CF10" s="9"/>
+      <c r="CG10" s="9"/>
+      <c r="CH10" s="9"/>
+      <c r="CI10" s="9"/>
+      <c r="CJ10" s="9"/>
+      <c r="CK10" s="9"/>
+      <c r="CL10" s="9"/>
+      <c r="CT10" s="9"/>
+      <c r="CW10" s="9"/>
+    </row>
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="BB11" s="9"/>
+      <c r="BE11" s="9"/>
+      <c r="CC11" s="9"/>
+      <c r="CD11" s="9"/>
+      <c r="CE11" s="9"/>
+      <c r="CF11" s="9"/>
+      <c r="CG11" s="9"/>
+      <c r="CH11" s="9"/>
+      <c r="CI11" s="9"/>
+      <c r="CJ11" s="9"/>
+      <c r="CK11" s="9"/>
+      <c r="CL11" s="9"/>
+      <c r="CT11" s="9"/>
+      <c r="CW11" s="9"/>
+    </row>
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
+      <c r="AT12" s="9"/>
+      <c r="BB12" s="9"/>
+      <c r="BE12" s="9"/>
+      <c r="CC12" s="9"/>
+      <c r="CD12" s="9"/>
+      <c r="CE12" s="9"/>
+      <c r="CF12" s="9"/>
+      <c r="CG12" s="9"/>
+      <c r="CH12" s="9"/>
+      <c r="CI12" s="9"/>
+      <c r="CJ12" s="9"/>
+      <c r="CK12" s="9"/>
+      <c r="CL12" s="9"/>
+      <c r="CT12" s="9"/>
+      <c r="CW12" s="9"/>
+    </row>
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
+      <c r="AN13" s="9"/>
+      <c r="AO13" s="9"/>
+      <c r="AP13" s="9"/>
+      <c r="AQ13" s="9"/>
+      <c r="AR13" s="9"/>
+      <c r="AS13" s="9"/>
+      <c r="AT13" s="9"/>
+      <c r="BB13" s="9"/>
+      <c r="BE13" s="9"/>
+      <c r="CC13" s="9"/>
+      <c r="CD13" s="9"/>
+      <c r="CE13" s="9"/>
+      <c r="CF13" s="9"/>
+      <c r="CG13" s="9"/>
+      <c r="CH13" s="9"/>
+      <c r="CI13" s="9"/>
+      <c r="CJ13" s="9"/>
+      <c r="CK13" s="9"/>
+      <c r="CL13" s="9"/>
+      <c r="CT13" s="9"/>
+      <c r="CW13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>